<commit_message>
saving field test data
</commit_message>
<xml_diff>
--- a/2022-02-28/_checklist.xlsx
+++ b/2022-02-28/_checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gits\gradys-raw-data\2022-02-28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0CBD9F-5C2A-4D03-B018-20BFC5F9565B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF5A9501-907D-422E-9447-007AC7745D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23532" yWindow="8772" windowWidth="9492" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre field" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Pre field'!$A$1:$C$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t>Type</t>
   </si>
@@ -199,6 +200,9 @@
   </si>
   <si>
     <t xml:space="preserve">Checar baterias dos 5 rádios </t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
@@ -566,19 +570,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>48</v>
       </c>
@@ -597,7 +601,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>48</v>
       </c>
@@ -608,7 +612,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>48</v>
       </c>
@@ -619,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -630,7 +634,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -641,8 +645,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>51</v>
       </c>
@@ -650,8 +656,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>51</v>
       </c>
@@ -659,8 +667,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>51</v>
       </c>
@@ -668,7 +678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
@@ -679,7 +689,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
         <v>5</v>
@@ -688,7 +698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
         <v>5</v>
@@ -697,7 +707,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
         <v>5</v>
@@ -706,7 +716,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
         <v>5</v>
@@ -715,7 +725,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
         <v>5</v>
@@ -724,7 +734,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -735,8 +745,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
@@ -744,7 +756,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -755,35 +767,35 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
         <v>6</v>
@@ -792,7 +804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
         <v>8</v>
@@ -801,7 +813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
@@ -810,7 +822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -821,7 +833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>48</v>
       </c>
@@ -832,7 +844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
         <v>9</v>
@@ -841,7 +853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
         <v>9</v>
@@ -850,92 +862,92 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -953,322 +965,330 @@
   </sheetPr>
   <dimension ref="A2:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="A2:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="1.6640625" customWidth="1"/>
-    <col min="3" max="3" width="88.6640625" customWidth="1"/>
+    <col min="2" max="2" width="1.6328125" customWidth="1"/>
+    <col min="3" max="3" width="88.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C5" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="C10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="C11" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="C12" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="C14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="C15" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="C17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="C18" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="C19" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="C20" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="C23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="C69" s="4"/>
     </row>
@@ -1284,7 +1304,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>